<commit_message>
Added tables on how the pi's look like. Also added some variations on varying the scales
</commit_message>
<xml_diff>
--- a/results/tables/cost_ratios.xlsx
+++ b/results/tables/cost_ratios.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DD1410-7DD6-4897-8277-1534DDE018E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D2FF6A-B0E6-4B7F-B0D0-170FA045E851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9380" yWindow="-21710" windowWidth="38620" windowHeight="21100" xr2:uid="{63219993-7418-4C2A-A490-10639D8BDF01}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{63219993-7418-4C2A-A490-10639D8BDF01}"/>
   </bookViews>
   <sheets>
-    <sheet name="v2" sheetId="2" r:id="rId1"/>
-    <sheet name="v1" sheetId="1" r:id="rId2"/>
+    <sheet name="v3" sheetId="3" r:id="rId1"/>
+    <sheet name="v2" sheetId="2" r:id="rId2"/>
+    <sheet name="v1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="25">
   <si>
     <t>r1</t>
   </si>
@@ -97,12 +98,27 @@
   <si>
     <t>Pooled 5-year differences</t>
   </si>
+  <si>
+    <t>Varying variables in index</t>
+  </si>
+  <si>
+    <t>brepeat-bme4</t>
+  </si>
+  <si>
+    <t>cplanme-bvariety</t>
+  </si>
+  <si>
+    <t>Pooled differences</t>
+  </si>
+  <si>
+    <t>5 year differences</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,8 +149,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +176,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -166,19 +195,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -190,7 +213,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -506,11 +538,1498 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE5BD11-D46C-4D79-9630-3CD0157F18EC}">
+  <dimension ref="A1:S27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:S1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="3.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+    </row>
+    <row r="2" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="K3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="G4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="K4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="Q4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R5" t="s">
+        <v>6</v>
+      </c>
+      <c r="S5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1">
+        <f t="shared" ref="G6:I8" si="0">+C6/$B6</f>
+        <v>1.7291666666666667</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5625</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="M6" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="1">
+        <f>+M6/$L6</f>
+        <v>9.45945945945946E-2</v>
+      </c>
+      <c r="R6" s="1">
+        <f>+N6/$L6</f>
+        <v>1.1621621621621621</v>
+      </c>
+      <c r="S6" s="1">
+        <f>+O6/$L6</f>
+        <v>1.1216216216216215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2542372881355932</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.81355932203389836</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1016949152542375</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="1">
+        <f>+M7/$L7</f>
+        <v>0.66101694915254239</v>
+      </c>
+      <c r="R7" s="1">
+        <f>+N7/$L7</f>
+        <v>1.2711864406779663</v>
+      </c>
+      <c r="S7" s="1">
+        <f>+O7/$L7</f>
+        <v>0.98305084745762705</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1754385964912282</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.9649122807017545</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.92982456140350889</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.41</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="1">
+        <f>+M8/$L8</f>
+        <v>0.63076923076923075</v>
+      </c>
+      <c r="R8" s="1">
+        <f>+N8/$L8</f>
+        <v>0.8</v>
+      </c>
+      <c r="S8" s="1">
+        <f>+O8/$L8</f>
+        <v>1.0923076923076922</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="K10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0.33</v>
+      </c>
+      <c r="C12">
+        <v>1.42</v>
+      </c>
+      <c r="D12">
+        <v>0.4</v>
+      </c>
+      <c r="E12">
+        <v>0.79</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1">
+        <f t="shared" ref="G12:I14" si="1">+C12/$B12</f>
+        <v>4.3030303030303028</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="1"/>
+        <v>1.2121212121212122</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="1"/>
+        <v>2.393939393939394</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="O12" s="2">
+        <v>1.29</v>
+      </c>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="1">
+        <f>+M12/$L12</f>
+        <v>1.3</v>
+      </c>
+      <c r="R12" s="1">
+        <f>+N12/$L12</f>
+        <v>1.02</v>
+      </c>
+      <c r="S12" s="1">
+        <f>+O12/$L12</f>
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C13">
+        <v>1.56</v>
+      </c>
+      <c r="D13">
+        <v>0.41</v>
+      </c>
+      <c r="E13">
+        <v>0.72</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1">
+        <f>+C13/$B13</f>
+        <v>2.6896551724137936</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.7068965517241379</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.2413793103448276</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.49</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="1">
+        <f>+M13/$L13</f>
+        <v>1.7755102040816326</v>
+      </c>
+      <c r="R13" s="1">
+        <f>+N13/$L13</f>
+        <v>1.7551020408163265</v>
+      </c>
+      <c r="S13" s="1">
+        <f>+O13/$L13</f>
+        <v>1.1020408163265307</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>0.71</v>
+      </c>
+      <c r="C14">
+        <v>1.38</v>
+      </c>
+      <c r="D14">
+        <v>0.49</v>
+      </c>
+      <c r="E14">
+        <v>0.67</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9436619718309858</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.6901408450704225</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.94366197183098599</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="M14" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="1">
+        <f>+M14/$L14</f>
+        <v>1.9811320754716981</v>
+      </c>
+      <c r="R14" s="1">
+        <f>+N14/$L14</f>
+        <v>0.96226415094339623</v>
+      </c>
+      <c r="S14" s="1">
+        <f>+O14/$L14</f>
+        <v>1.4716981132075471</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="K16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="G17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="K17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="Q17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" t="s">
+        <v>7</v>
+      </c>
+      <c r="L18" t="s">
+        <v>4</v>
+      </c>
+      <c r="M18" t="s">
+        <v>5</v>
+      </c>
+      <c r="N18" t="s">
+        <v>6</v>
+      </c>
+      <c r="O18" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>5</v>
+      </c>
+      <c r="R18" t="s">
+        <v>6</v>
+      </c>
+      <c r="S18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="1">
+        <f t="shared" ref="G19:G21" si="2">+C19/$B19</f>
+        <v>2.3404255319148941</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" ref="H19:H21" si="3">+D19/$B19</f>
+        <v>1.0851063829787235</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" ref="I19:I21" si="4">+E19/$B19</f>
+        <v>1.2553191489361701</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0.47</v>
+      </c>
+      <c r="M19">
+        <v>0.75</v>
+      </c>
+      <c r="N19">
+        <v>0.75</v>
+      </c>
+      <c r="O19">
+        <v>0.53</v>
+      </c>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="1">
+        <f>+M19/$L19</f>
+        <v>1.595744680851064</v>
+      </c>
+      <c r="R19" s="1">
+        <f>+N19/$L19</f>
+        <v>1.595744680851064</v>
+      </c>
+      <c r="S19" s="1">
+        <f>+O19/$L19</f>
+        <v>1.1276595744680853</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.41</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1.24</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="1">
+        <f t="shared" si="2"/>
+        <v>3.024390243902439</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="3"/>
+        <v>1.4634146341463414</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="4"/>
+        <v>1.0975609756097562</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>0.52</v>
+      </c>
+      <c r="M20">
+        <v>0.97</v>
+      </c>
+      <c r="N20">
+        <v>0.71</v>
+      </c>
+      <c r="O20">
+        <v>0.43</v>
+      </c>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="1">
+        <f>+M20/$L20</f>
+        <v>1.8653846153846152</v>
+      </c>
+      <c r="R20" s="1">
+        <f>+N20/$L20</f>
+        <v>1.3653846153846152</v>
+      </c>
+      <c r="S20" s="1">
+        <f>+O20/$L20</f>
+        <v>0.82692307692307687</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9259259259259258</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2592592592592593</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="4"/>
+        <v>0.79629629629629628</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21">
+        <v>0.52</v>
+      </c>
+      <c r="M21">
+        <v>1.03</v>
+      </c>
+      <c r="N21">
+        <v>0.59</v>
+      </c>
+      <c r="O21">
+        <v>0.52</v>
+      </c>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="1">
+        <f>+M21/$L21</f>
+        <v>1.9807692307692308</v>
+      </c>
+      <c r="R21" s="1">
+        <f>+N21/$L21</f>
+        <v>1.1346153846153846</v>
+      </c>
+      <c r="S21" s="1">
+        <f>+O21/$L21</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="K23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C25" s="2">
+        <v>3.48</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="1">
+        <f t="shared" ref="G25:G27" si="5">+C25/$B25</f>
+        <v>12.428571428571427</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" ref="H25:H27" si="6">+D25/$B25</f>
+        <v>1.5714285714285714</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" ref="I25:I27" si="7">+E25/$B25</f>
+        <v>1.3214285714285714</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="M25" s="2">
+        <v>2.97</v>
+      </c>
+      <c r="N25" s="2">
+        <v>0.69</v>
+      </c>
+      <c r="O25" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="1">
+        <f>+M25/$L25</f>
+        <v>49.500000000000007</v>
+      </c>
+      <c r="R25" s="1">
+        <f>+N25/$L25</f>
+        <v>11.5</v>
+      </c>
+      <c r="S25" s="1">
+        <f>+O25/$L25</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.41</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3.81</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="1">
+        <f>+C26/$B26</f>
+        <v>9.2926829268292686</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="6"/>
+        <v>1.1707317073170731</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="7"/>
+        <v>1.0975609756097562</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M26" s="2">
+        <v>2.34</v>
+      </c>
+      <c r="N26" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="O26" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="1">
+        <f>+M26/$L26</f>
+        <v>4.254545454545454</v>
+      </c>
+      <c r="R26" s="1">
+        <f>+N26/$L26</f>
+        <v>1.4909090909090907</v>
+      </c>
+      <c r="S26" s="1">
+        <f>+O26/$L26</f>
+        <v>0.67272727272727262</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="C27" s="2">
+        <v>3.19</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="1">
+        <f t="shared" ref="G27" si="8">+C27/$B27</f>
+        <v>4.5571428571428569</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="6"/>
+        <v>0.9571428571428573</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="7"/>
+        <v>0.68571428571428572</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="M27" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="N27" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="O27" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="1">
+        <f>+M27/$L27</f>
+        <v>4.7169811320754711</v>
+      </c>
+      <c r="R27" s="1">
+        <f>+N27/$L27</f>
+        <v>1.1132075471698113</v>
+      </c>
+      <c r="S27" s="1">
+        <f>+O27/$L27</f>
+        <v>1.2264150943396226</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="K2:S2"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="K3:S3"/>
+    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="K10:O10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="K16:S16"/>
+    <mergeCell ref="K17:O17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="G10:I10"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I6:I8">
+    <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6:H8">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6:G8">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12:I14">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:H14">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12:G14">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19:I21">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19:H21">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G19:G21">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25:I27">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25:H27">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G25:G27">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S15">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R15">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q15">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q25:Q27">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R25:R27">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S25:S27">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q19:Q21">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R19:R21">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S19:S21">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q12:Q14">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R12:R14">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S12:S14">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q6:Q8">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R6:R8">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S6:S8">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F7B63F-A290-42D1-99C0-83B7E9CF243F}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,44 +2038,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="G3" s="4" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="G3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -683,19 +2202,19 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
@@ -824,19 +2343,19 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
@@ -965,32 +2484,32 @@
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
@@ -1119,19 +2638,19 @@
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
@@ -1260,19 +2779,19 @@
       <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="8" t="s">
+      <c r="G34" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
@@ -1391,12 +2910,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="G28:I28"/>
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="G34:I34"/>
     <mergeCell ref="A3:E3"/>
@@ -1405,6 +2918,12 @@
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="G15:I15"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="G28:I28"/>
     <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:I7">
@@ -1651,7 +3170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4015DC4-F3A4-46CF-B24D-4D8E1466AFF5}">
   <dimension ref="A1:O37"/>
   <sheetViews>
@@ -1666,18 +3185,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="G1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="G1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
@@ -1815,18 +3334,18 @@
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="4" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="G8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
@@ -1967,18 +3486,18 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="G15" s="4" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="G15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
@@ -2085,18 +3604,18 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="G21" s="4" t="s">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="G21" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
@@ -2214,18 +3733,18 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="G27" s="4" t="s">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="G27" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
@@ -2332,18 +3851,18 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="G33" s="4" t="s">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="G33" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
@@ -2451,18 +3970,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="G33:I33"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="G33:I33"/>
   </mergeCells>
   <conditionalFormatting sqref="I17:I20">
     <cfRule type="colorScale" priority="15">

</xml_diff>

<commit_message>
Added average of log results
</commit_message>
<xml_diff>
--- a/results/tables/cost_ratios.xlsx
+++ b/results/tables/cost_ratios.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D2FF6A-B0E6-4B7F-B0D0-170FA045E851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A965177-EB2E-47ED-9AE5-50AAD86E6AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{63219993-7418-4C2A-A490-10639D8BDF01}"/>
   </bookViews>
   <sheets>
-    <sheet name="v3" sheetId="3" r:id="rId1"/>
-    <sheet name="v2" sheetId="2" r:id="rId2"/>
-    <sheet name="v1" sheetId="1" r:id="rId3"/>
+    <sheet name="v4" sheetId="4" r:id="rId1"/>
+    <sheet name="v3" sheetId="3" r:id="rId2"/>
+    <sheet name="v2" sheetId="2" r:id="rId3"/>
+    <sheet name="v1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="27">
   <si>
     <t>r1</t>
   </si>
@@ -112,6 +113,12 @@
   </si>
   <si>
     <t>5 year differences</t>
+  </si>
+  <si>
+    <t>educ_3_mid asinh(average)</t>
+  </si>
+  <si>
+    <t>educ_3_mid average(asinh)</t>
   </si>
 </sst>
 </file>
@@ -195,17 +202,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -213,16 +221,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -538,11 +546,456 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{321D5AB5-D874-47B9-AD75-84BA75D75E3A}">
+  <dimension ref="A1:S15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="3.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+    </row>
+    <row r="2" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="G4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1">
+        <f t="shared" ref="G6:I8" si="0">+C6/$B6</f>
+        <v>1.7291666666666667</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2542372881355932</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.81355932203389836</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1016949152542375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1754385964912282</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.9649122807017545</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.92982456140350889</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1">
+        <f t="shared" ref="G12:I14" si="1">+C12/$B12</f>
+        <v>2.8249999999999997</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5499999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1">
+        <f>+C13/$B13</f>
+        <v>2.5813953488372094</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1162790697674418</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.2093023255813955</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9215686274509802</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0784313725490198</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.94117647058823528</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="G10:I10"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I6:I8">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6:H8">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6:G8">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12:I14">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:H14">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12:G14">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE5BD11-D46C-4D79-9630-3CD0157F18EC}">
   <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:S1"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -574,78 +1027,78 @@
       <c r="S1" s="10"/>
     </row>
     <row r="2" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="K2" s="4" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="K2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="K3" s="9" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="K3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="G4" s="8" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="G4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="K4" s="7" t="s">
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="K4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="Q4" s="8" t="s">
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="Q4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
@@ -737,15 +1190,15 @@
       </c>
       <c r="P6" s="2"/>
       <c r="Q6" s="1">
-        <f>+M6/$L6</f>
+        <f t="shared" ref="Q6:S8" si="1">+M6/$L6</f>
         <v>9.45945945945946E-2</v>
       </c>
       <c r="R6" s="1">
-        <f>+N6/$L6</f>
+        <f t="shared" si="1"/>
         <v>1.1621621621621621</v>
       </c>
       <c r="S6" s="1">
-        <f>+O6/$L6</f>
+        <f t="shared" si="1"/>
         <v>1.1216216216216215</v>
       </c>
     </row>
@@ -795,15 +1248,15 @@
       </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="1">
-        <f>+M7/$L7</f>
+        <f t="shared" si="1"/>
         <v>0.66101694915254239</v>
       </c>
       <c r="R7" s="1">
-        <f>+N7/$L7</f>
+        <f t="shared" si="1"/>
         <v>1.2711864406779663</v>
       </c>
       <c r="S7" s="1">
-        <f>+O7/$L7</f>
+        <f t="shared" si="1"/>
         <v>0.98305084745762705</v>
       </c>
     </row>
@@ -853,15 +1306,15 @@
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="1">
-        <f>+M8/$L8</f>
+        <f t="shared" si="1"/>
         <v>0.63076923076923075</v>
       </c>
       <c r="R8" s="1">
-        <f>+N8/$L8</f>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="S8" s="1">
-        <f>+O8/$L8</f>
+        <f t="shared" si="1"/>
         <v>1.0923076923076922</v>
       </c>
     </row>
@@ -886,32 +1339,32 @@
       <c r="S9" s="2"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="K10" s="5" t="s">
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="K10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
       <c r="P10" s="2"/>
-      <c r="Q10" s="6" t="s">
+      <c r="Q10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
@@ -979,15 +1432,15 @@
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="1">
-        <f t="shared" ref="G12:I14" si="1">+C12/$B12</f>
+        <f t="shared" ref="G12:I14" si="2">+C12/$B12</f>
         <v>4.3030303030303028</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2121212121212122</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.393939393939394</v>
       </c>
       <c r="K12" s="2" t="s">
@@ -1007,15 +1460,15 @@
       </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="1">
-        <f>+M12/$L12</f>
+        <f t="shared" ref="Q12:S14" si="3">+M12/$L12</f>
         <v>1.3</v>
       </c>
       <c r="R12" s="1">
-        <f>+N12/$L12</f>
+        <f t="shared" si="3"/>
         <v>1.02</v>
       </c>
       <c r="S12" s="1">
-        <f>+O12/$L12</f>
+        <f t="shared" si="3"/>
         <v>2.58</v>
       </c>
     </row>
@@ -1041,11 +1494,11 @@
         <v>2.6896551724137936</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.7068965517241379</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2413793103448276</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -1065,15 +1518,15 @@
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" s="1">
-        <f>+M13/$L13</f>
+        <f t="shared" si="3"/>
         <v>1.7755102040816326</v>
       </c>
       <c r="R13" s="1">
-        <f>+N13/$L13</f>
+        <f t="shared" si="3"/>
         <v>1.7551020408163265</v>
       </c>
       <c r="S13" s="1">
-        <f>+O13/$L13</f>
+        <f t="shared" si="3"/>
         <v>1.1020408163265307</v>
       </c>
     </row>
@@ -1095,15 +1548,15 @@
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.9436619718309858</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.6901408450704225</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.94366197183098599</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -1123,15 +1576,15 @@
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="1">
-        <f>+M14/$L14</f>
+        <f t="shared" si="3"/>
         <v>1.9811320754716981</v>
       </c>
       <c r="R14" s="1">
-        <f>+N14/$L14</f>
+        <f t="shared" si="3"/>
         <v>0.96226415094339623</v>
       </c>
       <c r="S14" s="1">
-        <f>+O14/$L14</f>
+        <f t="shared" si="3"/>
         <v>1.4716981132075471</v>
       </c>
     </row>
@@ -1156,54 +1609,54 @@
       <c r="S15" s="2"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="K16" s="9" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="K16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="G17" s="8" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="G17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="K17" s="7" t="s">
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="K17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="Q17" s="8" t="s">
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="Q17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
@@ -1267,15 +1720,15 @@
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="1">
-        <f t="shared" ref="G19:G21" si="2">+C19/$B19</f>
+        <f t="shared" ref="G19:G21" si="4">+C19/$B19</f>
         <v>2.3404255319148941</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" ref="H19:H21" si="3">+D19/$B19</f>
+        <f t="shared" ref="H19:H21" si="5">+D19/$B19</f>
         <v>1.0851063829787235</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" ref="I19:I21" si="4">+E19/$B19</f>
+        <f t="shared" ref="I19:I21" si="6">+E19/$B19</f>
         <v>1.2553191489361701</v>
       </c>
       <c r="K19" s="2" t="s">
@@ -1295,15 +1748,15 @@
       </c>
       <c r="P19" s="2"/>
       <c r="Q19" s="1">
-        <f>+M19/$L19</f>
+        <f t="shared" ref="Q19:S21" si="7">+M19/$L19</f>
         <v>1.595744680851064</v>
       </c>
       <c r="R19" s="1">
-        <f>+N19/$L19</f>
+        <f t="shared" si="7"/>
         <v>1.595744680851064</v>
       </c>
       <c r="S19" s="1">
-        <f>+O19/$L19</f>
+        <f t="shared" si="7"/>
         <v>1.1276595744680853</v>
       </c>
     </row>
@@ -1325,15 +1778,15 @@
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.024390243902439</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.4634146341463414</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0975609756097562</v>
       </c>
       <c r="K20" s="2" t="s">
@@ -1353,15 +1806,15 @@
       </c>
       <c r="P20" s="2"/>
       <c r="Q20" s="1">
-        <f>+M20/$L20</f>
+        <f t="shared" si="7"/>
         <v>1.8653846153846152</v>
       </c>
       <c r="R20" s="1">
-        <f>+N20/$L20</f>
+        <f t="shared" si="7"/>
         <v>1.3653846153846152</v>
       </c>
       <c r="S20" s="1">
-        <f>+O20/$L20</f>
+        <f t="shared" si="7"/>
         <v>0.82692307692307687</v>
       </c>
     </row>
@@ -1383,15 +1836,15 @@
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9259259259259258</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.2592592592592593</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.79629629629629628</v>
       </c>
       <c r="K21" s="2" t="s">
@@ -1411,15 +1864,15 @@
       </c>
       <c r="P21" s="2"/>
       <c r="Q21" s="1">
-        <f>+M21/$L21</f>
+        <f t="shared" si="7"/>
         <v>1.9807692307692308</v>
       </c>
       <c r="R21" s="1">
-        <f>+N21/$L21</f>
+        <f t="shared" si="7"/>
         <v>1.1346153846153846</v>
       </c>
       <c r="S21" s="1">
-        <f>+O21/$L21</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -1444,32 +1897,32 @@
       <c r="S22" s="2"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="K23" s="5" t="s">
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="K23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
       <c r="P23" s="2"/>
-      <c r="Q23" s="6" t="s">
+      <c r="Q23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="R23" s="6"/>
-      <c r="S23" s="6"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
@@ -1537,15 +1990,15 @@
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="1">
-        <f t="shared" ref="G25:G27" si="5">+C25/$B25</f>
+        <f t="shared" ref="G25" si="8">+C25/$B25</f>
         <v>12.428571428571427</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" ref="H25:H27" si="6">+D25/$B25</f>
+        <f t="shared" ref="H25:H27" si="9">+D25/$B25</f>
         <v>1.5714285714285714</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" ref="I25:I27" si="7">+E25/$B25</f>
+        <f t="shared" ref="I25:I27" si="10">+E25/$B25</f>
         <v>1.3214285714285714</v>
       </c>
       <c r="K25" s="2" t="s">
@@ -1565,15 +2018,15 @@
       </c>
       <c r="P25" s="2"/>
       <c r="Q25" s="1">
-        <f>+M25/$L25</f>
+        <f t="shared" ref="Q25:S27" si="11">+M25/$L25</f>
         <v>49.500000000000007</v>
       </c>
       <c r="R25" s="1">
-        <f>+N25/$L25</f>
+        <f t="shared" si="11"/>
         <v>11.5</v>
       </c>
       <c r="S25" s="1">
-        <f>+O25/$L25</f>
+        <f t="shared" si="11"/>
         <v>1.5</v>
       </c>
     </row>
@@ -1599,11 +2052,11 @@
         <v>9.2926829268292686</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.1707317073170731</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1.0975609756097562</v>
       </c>
       <c r="K26" s="2" t="s">
@@ -1623,15 +2076,15 @@
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" s="1">
-        <f>+M26/$L26</f>
+        <f t="shared" si="11"/>
         <v>4.254545454545454</v>
       </c>
       <c r="R26" s="1">
-        <f>+N26/$L26</f>
+        <f t="shared" si="11"/>
         <v>1.4909090909090907</v>
       </c>
       <c r="S26" s="1">
-        <f>+O26/$L26</f>
+        <f t="shared" si="11"/>
         <v>0.67272727272727262</v>
       </c>
     </row>
@@ -1653,15 +2106,15 @@
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="1">
-        <f t="shared" ref="G27" si="8">+C27/$B27</f>
+        <f t="shared" ref="G27" si="12">+C27/$B27</f>
         <v>4.5571428571428569</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.9571428571428573</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.68571428571428572</v>
       </c>
       <c r="K27" s="2" t="s">
@@ -1681,15 +2134,15 @@
       </c>
       <c r="P27" s="2"/>
       <c r="Q27" s="1">
-        <f>+M27/$L27</f>
+        <f t="shared" si="11"/>
         <v>4.7169811320754711</v>
       </c>
       <c r="R27" s="1">
-        <f>+N27/$L27</f>
+        <f t="shared" si="11"/>
         <v>1.1132075471698113</v>
       </c>
       <c r="S27" s="1">
-        <f>+O27/$L27</f>
+        <f t="shared" si="11"/>
         <v>1.2264150943396226</v>
       </c>
     </row>
@@ -2024,7 +2477,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F7B63F-A290-42D1-99C0-83B7E9CF243F}">
   <dimension ref="A1:I38"/>
   <sheetViews>
@@ -2038,44 +2491,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="G3" s="8" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="G3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -2202,19 +2655,19 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
@@ -2343,19 +2796,19 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
@@ -2484,32 +2937,32 @@
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
@@ -2638,19 +3091,19 @@
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="6" t="s">
+      <c r="G28" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
@@ -2779,19 +3232,19 @@
       <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="6" t="s">
+      <c r="G34" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
@@ -3170,7 +3623,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4015DC4-F3A4-46CF-B24D-4D8E1466AFF5}">
   <dimension ref="A1:O37"/>
   <sheetViews>
@@ -3185,18 +3638,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="G1" s="8" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="G1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
@@ -3334,18 +3787,18 @@
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="G8" s="8" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="G8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
@@ -3486,18 +3939,18 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="G15" s="8" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="G15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
@@ -3604,18 +4057,18 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="G21" s="8" t="s">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="G21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
@@ -3733,18 +4186,18 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="G27" s="8" t="s">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="G27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
@@ -3851,18 +4304,18 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="G33" s="8" t="s">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="G33" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B34" t="s">

</xml_diff>

<commit_message>
Readded sum of skills sum to 1. Not nice results
</commit_message>
<xml_diff>
--- a/results/tables/cost_ratios.xlsx
+++ b/results/tables/cost_ratios.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A965177-EB2E-47ED-9AE5-50AAD86E6AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC145832-0AE0-4170-901B-DA0A3F0B1743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{63219993-7418-4C2A-A490-10639D8BDF01}"/>
   </bookViews>
   <sheets>
-    <sheet name="v4" sheetId="4" r:id="rId1"/>
-    <sheet name="v3" sheetId="3" r:id="rId2"/>
-    <sheet name="v2" sheetId="2" r:id="rId3"/>
-    <sheet name="v1" sheetId="1" r:id="rId4"/>
+    <sheet name="v6" sheetId="6" r:id="rId1"/>
+    <sheet name="v5" sheetId="5" r:id="rId2"/>
+    <sheet name="v4" sheetId="4" r:id="rId3"/>
+    <sheet name="v3" sheetId="3" r:id="rId4"/>
+    <sheet name="v2" sheetId="2" r:id="rId5"/>
+    <sheet name="v1" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="38">
   <si>
     <t>r1</t>
   </si>
@@ -119,6 +122,39 @@
   </si>
   <si>
     <t>educ_3_mid average(asinh)</t>
+  </si>
+  <si>
+    <t>educ_3_low average(asinh)</t>
+  </si>
+  <si>
+    <t>manual</t>
+  </si>
+  <si>
+    <t>routine</t>
+  </si>
+  <si>
+    <t>social</t>
+  </si>
+  <si>
+    <t>abstract</t>
+  </si>
+  <si>
+    <t>educ_4 average(asinh)</t>
+  </si>
+  <si>
+    <t>Lower GCSE</t>
+  </si>
+  <si>
+    <t>Higher GCSE</t>
+  </si>
+  <si>
+    <t>A* levels</t>
+  </si>
+  <si>
+    <t>Colleges</t>
+  </si>
+  <si>
+    <t>Cost ratios (reference:routine)</t>
   </si>
 </sst>
 </file>
@@ -209,6 +245,12 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -220,12 +262,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -546,11 +582,858 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C60D7FD-9683-4F3F-ACC9-67E02816B2AB}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="G3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>0.4</v>
+      </c>
+      <c r="C5">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.33</v>
+      </c>
+      <c r="E5">
+        <v>0.65</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="1">
+        <f>+B5/$C5</f>
+        <v>0.34482758620689657</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" ref="H5:I8" si="0">+D5/$C5</f>
+        <v>0.28448275862068967</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.56034482758620696</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>0.49</v>
+      </c>
+      <c r="C6">
+        <v>1.01</v>
+      </c>
+      <c r="D6">
+        <v>0.49</v>
+      </c>
+      <c r="E6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1">
+        <f>+B6/$C6</f>
+        <v>0.48514851485148514</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.48514851485148514</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5544554455445545</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <v>0.32</v>
+      </c>
+      <c r="C7">
+        <v>0.99</v>
+      </c>
+      <c r="D7">
+        <v>0.52</v>
+      </c>
+      <c r="E7">
+        <v>0.53</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1">
+        <f>+B7/$C7</f>
+        <v>0.32323232323232326</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5252525252525253</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.53535353535353536</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8">
+        <v>0.53</v>
+      </c>
+      <c r="C8">
+        <v>0.96</v>
+      </c>
+      <c r="D8">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E8">
+        <v>0.47</v>
+      </c>
+      <c r="G8" s="1">
+        <f>+B8/$C8</f>
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.59375</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.48958333333333331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1">
+        <f>+B12/$C12</f>
+        <v>0.3539823008849558</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" ref="H12:I14" si="1">+D12/$C12</f>
+        <v>0.33628318584070799</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.54867256637168149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1">
+        <f>+B13/$C13</f>
+        <v>0.38738738738738737</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.4324324324324324</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.46846846846846846</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="1">
+        <f>+B14/$C14</f>
+        <v>0.52040816326530615</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.56122448979591844</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.48979591836734693</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="G10:I10"/>
+  </mergeCells>
+  <conditionalFormatting sqref="G5:G8">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H8">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:I8">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12:G14">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:H14">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12:I14">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E114E29E-6676-4C6A-A5B1-6F74E9DDBA1A}">
+  <dimension ref="A1:P13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="G3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.06</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.61</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="1">
+        <f>+C5/$B5</f>
+        <v>2.3043478260869565</v>
+      </c>
+      <c r="H5" s="1">
+        <f>+D5/$B5</f>
+        <v>0.9565217391304347</v>
+      </c>
+      <c r="I5" s="1">
+        <f>+E5/$B5</f>
+        <v>1.326086956521739</v>
+      </c>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1">
+        <f t="shared" ref="G6:I7" si="0">+C6/$B6</f>
+        <v>4</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I6" s="1">
+        <f>+E6/$B6</f>
+        <v>1.9230769230769229</v>
+      </c>
+      <c r="L6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0.4</v>
+      </c>
+      <c r="N6">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="O6">
+        <v>0.33</v>
+      </c>
+      <c r="P6">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.96</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.04</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0.49</v>
+      </c>
+      <c r="N7">
+        <v>1.01</v>
+      </c>
+      <c r="O7">
+        <v>0.49</v>
+      </c>
+      <c r="P7">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="L8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>0.32</v>
+      </c>
+      <c r="N8">
+        <v>0.99</v>
+      </c>
+      <c r="O8">
+        <v>0.52</v>
+      </c>
+      <c r="P8">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="L9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>0.53</v>
+      </c>
+      <c r="N9">
+        <v>0.96</v>
+      </c>
+      <c r="O9">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="P9">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="1">
+        <f t="shared" ref="G11:I13" si="1">+C11/$B11</f>
+        <v>2.8249999999999997</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5499999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1">
+        <f>+C12/$B12</f>
+        <v>2.5813953488372094</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1162790697674418</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="1"/>
+        <v>1.2093023255813955</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1">
+        <f>+C13/$B13</f>
+        <v>1.9215686274509802</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0784313725490198</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.94117647058823528</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="G9:I9"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I5:I7">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H7">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G7">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11:I13">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11:H13">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:G13">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{321D5AB5-D874-47B9-AD75-84BA75D75E3A}">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -582,44 +1465,44 @@
       <c r="S1" s="3"/>
     </row>
     <row r="2" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="G4" s="5" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="G4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
@@ -746,19 +1629,19 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
@@ -888,13 +1771,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="G10:I10"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="G4:I4"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="G10:I10"/>
   </mergeCells>
   <conditionalFormatting sqref="I6:I8">
     <cfRule type="colorScale" priority="30">
@@ -990,7 +1873,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE5BD11-D46C-4D79-9630-3CD0157F18EC}">
   <dimension ref="A1:S27"/>
   <sheetViews>
@@ -1027,78 +1910,78 @@
       <c r="S1" s="10"/>
     </row>
     <row r="2" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="K2" s="9" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="K3" s="8" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="K3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="G4" s="5" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="G4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="K4" s="4" t="s">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="K4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="Q4" s="5" t="s">
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="Q4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
@@ -1339,32 +2222,32 @@
       <c r="S9" s="2"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="K10" s="6" t="s">
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="K10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
       <c r="P10" s="2"/>
-      <c r="Q10" s="7" t="s">
+      <c r="Q10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
@@ -1609,54 +2492,54 @@
       <c r="S15" s="2"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="K16" s="8" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="K16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="G17" s="5" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="G17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="K17" s="4" t="s">
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="K17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="Q17" s="5" t="s">
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="Q17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
@@ -1720,15 +2603,15 @@
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="1">
-        <f t="shared" ref="G19:G21" si="4">+C19/$B19</f>
+        <f t="shared" ref="G19:I21" si="4">+C19/$B19</f>
         <v>2.3404255319148941</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" ref="H19:H21" si="5">+D19/$B19</f>
+        <f t="shared" si="4"/>
         <v>1.0851063829787235</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" ref="I19:I21" si="6">+E19/$B19</f>
+        <f t="shared" si="4"/>
         <v>1.2553191489361701</v>
       </c>
       <c r="K19" s="2" t="s">
@@ -1748,15 +2631,15 @@
       </c>
       <c r="P19" s="2"/>
       <c r="Q19" s="1">
-        <f t="shared" ref="Q19:S21" si="7">+M19/$L19</f>
+        <f t="shared" ref="Q19:S21" si="5">+M19/$L19</f>
         <v>1.595744680851064</v>
       </c>
       <c r="R19" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.595744680851064</v>
       </c>
       <c r="S19" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.1276595744680853</v>
       </c>
     </row>
@@ -1782,11 +2665,11 @@
         <v>3.024390243902439</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.4634146341463414</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.0975609756097562</v>
       </c>
       <c r="K20" s="2" t="s">
@@ -1806,15 +2689,15 @@
       </c>
       <c r="P20" s="2"/>
       <c r="Q20" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.8653846153846152</v>
       </c>
       <c r="R20" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.3653846153846152</v>
       </c>
       <c r="S20" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0.82692307692307687</v>
       </c>
     </row>
@@ -1840,11 +2723,11 @@
         <v>1.9259259259259258</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.2592592592592593</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.79629629629629628</v>
       </c>
       <c r="K21" s="2" t="s">
@@ -1864,15 +2747,15 @@
       </c>
       <c r="P21" s="2"/>
       <c r="Q21" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.9807692307692308</v>
       </c>
       <c r="R21" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.1346153846153846</v>
       </c>
       <c r="S21" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -1897,32 +2780,32 @@
       <c r="S22" s="2"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="K23" s="6" t="s">
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="K23" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
       <c r="P23" s="2"/>
-      <c r="Q23" s="7" t="s">
+      <c r="Q23" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
@@ -1990,15 +2873,15 @@
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="1">
-        <f t="shared" ref="G25" si="8">+C25/$B25</f>
+        <f t="shared" ref="G25:I27" si="6">+C25/$B25</f>
         <v>12.428571428571427</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" ref="H25:H27" si="9">+D25/$B25</f>
+        <f t="shared" si="6"/>
         <v>1.5714285714285714</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" ref="I25:I27" si="10">+E25/$B25</f>
+        <f t="shared" si="6"/>
         <v>1.3214285714285714</v>
       </c>
       <c r="K25" s="2" t="s">
@@ -2018,15 +2901,15 @@
       </c>
       <c r="P25" s="2"/>
       <c r="Q25" s="1">
-        <f t="shared" ref="Q25:S27" si="11">+M25/$L25</f>
+        <f t="shared" ref="Q25:S27" si="7">+M25/$L25</f>
         <v>49.500000000000007</v>
       </c>
       <c r="R25" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>11.5</v>
       </c>
       <c r="S25" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>1.5</v>
       </c>
     </row>
@@ -2048,15 +2931,15 @@
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="1">
-        <f>+C26/$B26</f>
+        <f t="shared" si="6"/>
         <v>9.2926829268292686</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>1.1707317073170731</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>1.0975609756097562</v>
       </c>
       <c r="K26" s="2" t="s">
@@ -2076,15 +2959,15 @@
       </c>
       <c r="P26" s="2"/>
       <c r="Q26" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>4.254545454545454</v>
       </c>
       <c r="R26" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>1.4909090909090907</v>
       </c>
       <c r="S26" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0.67272727272727262</v>
       </c>
     </row>
@@ -2106,15 +2989,15 @@
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="1">
-        <f t="shared" ref="G27" si="12">+C27/$B27</f>
+        <f t="shared" si="6"/>
         <v>4.5571428571428569</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0.9571428571428573</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0.68571428571428572</v>
       </c>
       <c r="K27" s="2" t="s">
@@ -2134,20 +3017,27 @@
       </c>
       <c r="P27" s="2"/>
       <c r="Q27" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>4.7169811320754711</v>
       </c>
       <c r="R27" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>1.1132075471698113</v>
       </c>
       <c r="S27" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>1.2264150943396226</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="G10:I10"/>
     <mergeCell ref="K23:O23"/>
     <mergeCell ref="Q23:S23"/>
     <mergeCell ref="K2:S2"/>
@@ -2164,13 +3054,6 @@
     <mergeCell ref="Q17:S17"/>
     <mergeCell ref="A16:I16"/>
     <mergeCell ref="A17:E17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="G10:I10"/>
   </mergeCells>
   <conditionalFormatting sqref="I6:I8">
     <cfRule type="colorScale" priority="50">
@@ -2477,7 +3360,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F7B63F-A290-42D1-99C0-83B7E9CF243F}">
   <dimension ref="A1:I38"/>
   <sheetViews>
@@ -2491,44 +3374,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="G3" s="5" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="G3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -2655,19 +3538,19 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
@@ -2712,15 +3595,15 @@
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="1">
-        <f t="shared" ref="G11:G13" si="1">+C11/$B11</f>
+        <f t="shared" ref="G11:I13" si="1">+C11/$B11</f>
         <v>12.210526315789473</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" ref="H11:H13" si="2">+D11/$B11</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" ref="I11:I13" si="3">+E11/$B11</f>
+        <f t="shared" si="1"/>
         <v>2.8421052631578947</v>
       </c>
     </row>
@@ -2742,15 +3625,15 @@
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="1">
-        <f>+C12/$B12</f>
+        <f t="shared" si="1"/>
         <v>6.0750000000000002</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.4749999999999999</v>
       </c>
     </row>
@@ -2776,11 +3659,11 @@
         <v>4</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.92857142857142849</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.9821428571428571</v>
       </c>
     </row>
@@ -2796,19 +3679,19 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
@@ -2853,15 +3736,15 @@
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="1">
-        <f t="shared" ref="G17:G19" si="4">+C17/$B17</f>
+        <f t="shared" ref="G17:I19" si="2">+C17/$B17</f>
         <v>3.375</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" ref="H17:H19" si="5">+D17/$B17</f>
+        <f t="shared" si="2"/>
         <v>1.375</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" ref="I17:I19" si="6">+E17/$B17</f>
+        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
     </row>
@@ -2883,15 +3766,15 @@
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3.375</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1.625</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>2.125</v>
       </c>
     </row>
@@ -2913,15 +3796,15 @@
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.9090909090909089</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1.5454545454545456</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>1.4545454545454546</v>
       </c>
     </row>
@@ -2950,19 +3833,19 @@
       <c r="I21" s="11"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
@@ -3007,15 +3890,15 @@
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="1">
-        <f t="shared" ref="G24:G26" si="7">+C24/$B24</f>
+        <f t="shared" ref="G24:I26" si="3">+C24/$B24</f>
         <v>0.6724137931034484</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" ref="H24:H26" si="8">+D24/$B24</f>
+        <f t="shared" si="3"/>
         <v>1.2931034482758621</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" ref="I24:I26" si="9">+E24/$B24</f>
+        <f t="shared" si="3"/>
         <v>1.2586206896551724</v>
       </c>
     </row>
@@ -3037,15 +3920,15 @@
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>1.68</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>1.32</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>0.92</v>
       </c>
     </row>
@@ -3067,15 +3950,15 @@
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>1.7450980392156863</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>0.98039215686274506</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>1.1176470588235292</v>
       </c>
     </row>
@@ -3091,19 +3974,19 @@
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="7" t="s">
+      <c r="G28" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
@@ -3148,15 +4031,15 @@
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="1">
-        <f t="shared" ref="G30:G32" si="10">+C30/$B30</f>
+        <f t="shared" ref="G30:I32" si="4">+C30/$B30</f>
         <v>6.875</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" ref="H30:H32" si="11">+D30/$B30</f>
+        <f t="shared" si="4"/>
         <v>1.9166666666666667</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" ref="I30:I32" si="12">+E30/$B30</f>
+        <f t="shared" si="4"/>
         <v>3.3750000000000004</v>
       </c>
     </row>
@@ -3178,15 +4061,15 @@
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>4.4146341463414638</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>1.7560975609756098</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>0.92682926829268297</v>
       </c>
     </row>
@@ -3208,15 +4091,15 @@
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>5.2631578947368425</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>1.263157894736842</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>1.7105263157894737</v>
       </c>
     </row>
@@ -3232,19 +4115,19 @@
       <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="7" t="s">
+      <c r="G34" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
@@ -3289,15 +4172,15 @@
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="1">
-        <f t="shared" ref="G36:G38" si="13">+C36/$B36</f>
+        <f t="shared" ref="G36:I38" si="5">+C36/$B36</f>
         <v>1.7</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" ref="H36:H38" si="14">+D36/$B36</f>
+        <f t="shared" si="5"/>
         <v>1.7</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" ref="I36:I38" si="15">+E36/$B36</f>
+        <f t="shared" si="5"/>
         <v>2.1999999999999997</v>
       </c>
     </row>
@@ -3319,15 +4202,15 @@
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="5"/>
         <v>1.4615384615384615</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.5384615384615385</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>1.2307692307692308</v>
       </c>
     </row>
@@ -3349,20 +4232,26 @@
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="5"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="H38" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.1666666666666667</v>
       </c>
       <c r="I38" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>1.75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="A2:I2"/>
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="G34:I34"/>
     <mergeCell ref="A3:E3"/>
@@ -3372,12 +4261,6 @@
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="G15:I15"/>
     <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="A2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:I7">
     <cfRule type="colorScale" priority="27">
@@ -3623,7 +4506,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4015DC4-F3A4-46CF-B24D-4D8E1466AFF5}">
   <dimension ref="A1:O37"/>
   <sheetViews>
@@ -3638,18 +4521,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="G1" s="5" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="G1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
@@ -3682,11 +4565,11 @@
         <v>0.83</v>
       </c>
       <c r="G3" s="1">
-        <f>+C3/$B3</f>
+        <f t="shared" ref="G3:I6" si="0">+C3/$B3</f>
         <v>0.30337078651685395</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:I3" si="0">+D3/$B3</f>
+        <f t="shared" si="0"/>
         <v>0.8314606741573034</v>
       </c>
       <c r="I3" s="1">
@@ -3711,15 +4594,15 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" ref="G4:G6" si="1">+C4/$B4</f>
+        <f t="shared" si="0"/>
         <v>0.52542372881355937</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H6" si="2">+D4/$B4</f>
+        <f t="shared" si="0"/>
         <v>0.20338983050847459</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" ref="I4:I6" si="3">+E4/$B4</f>
+        <f t="shared" si="0"/>
         <v>0.93220338983050854</v>
       </c>
     </row>
@@ -3740,15 +4623,15 @@
         <v>0.76</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.16161616161616163</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.71717171717171713</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.76767676767676774</v>
       </c>
     </row>
@@ -3769,15 +4652,15 @@
         <v>0.72</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.23008849557522126</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.54867256637168149</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.63716814159292035</v>
       </c>
     </row>
@@ -3787,18 +4670,18 @@
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="G8" s="5" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="G8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
@@ -3834,15 +4717,15 @@
         <v>0.6</v>
       </c>
       <c r="G10" s="1">
-        <f>+C10/$B10</f>
+        <f t="shared" ref="G10:I13" si="1">+C10/$B10</f>
         <v>3.1052631578947367</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" ref="H10:H13" si="4">+D10/$B10</f>
+        <f t="shared" si="1"/>
         <v>0.94736842105263153</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" ref="I10:I12" si="5">+E10/$B10</f>
+        <f t="shared" si="1"/>
         <v>1.5789473684210527</v>
       </c>
     </row>
@@ -3863,15 +4746,15 @@
         <v>0.5</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" ref="G11:G13" si="6">+C11/$B11</f>
+        <f t="shared" si="1"/>
         <v>2.1956521739130435</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1.173913043478261</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
       </c>
     </row>
@@ -3892,15 +4775,15 @@
         <v>0.49</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1.8333333333333335</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>1.6333333333333333</v>
       </c>
     </row>
@@ -3921,15 +4804,15 @@
         <v>0.44</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>1.8627450980392155</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1.1764705882352942</v>
       </c>
       <c r="I13" s="1">
-        <f>+E13/$B13</f>
+        <f t="shared" si="1"/>
         <v>0.86274509803921573</v>
       </c>
     </row>
@@ -3939,18 +4822,18 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="G15" s="5" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="G15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
@@ -3986,15 +4869,15 @@
         <v>0.62</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" ref="G17:I19" si="7">+C17/$B17</f>
+        <f t="shared" ref="G17:I19" si="2">+C17/$B17</f>
         <v>1.4347826086956521</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>1.3913043478260869</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>1.3478260869565217</v>
       </c>
     </row>
@@ -4015,15 +4898,15 @@
         <v>0.46</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>1.6190476190476193</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>1.7619047619047619</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>1.0952380952380953</v>
       </c>
     </row>
@@ -4044,31 +4927,31 @@
         <v>0.48</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>1.1136363636363635</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>1.6818181818181819</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>1.0909090909090908</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="G21" s="5" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="G21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
@@ -4104,15 +4987,15 @@
         <v>0.66</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" ref="G23:I25" si="8">+C23/$B23</f>
+        <f t="shared" ref="G23:I25" si="3">+C23/$B23</f>
         <v>2.7837837837837838</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>0.86486486486486491</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>1.783783783783784</v>
       </c>
     </row>
@@ -4133,15 +5016,15 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>2.8055555555555558</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>1.1666666666666667</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>1.5277777777777779</v>
       </c>
       <c r="O24">
@@ -4165,15 +5048,15 @@
         <v>0.62</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>2.0888888888888886</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>0.84444444444444444</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>1.3777777777777778</v>
       </c>
       <c r="O25">
@@ -4186,18 +5069,18 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="G27" s="5" t="s">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="G27" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
@@ -4233,15 +5116,15 @@
         <v>0.42</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" ref="G29:I31" si="9">+C29/$B29</f>
+        <f t="shared" ref="G29:I31" si="4">+C29/$B29</f>
         <v>1.5813953488372094</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>1.8372093023255816</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>0.97674418604651159</v>
       </c>
     </row>
@@ -4262,15 +5145,15 @@
         <v>0.32</v>
       </c>
       <c r="G30" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>2.9090909090909092</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>3.9090909090909092</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>1.4545454545454546</v>
       </c>
     </row>
@@ -4291,31 +5174,31 @@
         <v>0.52</v>
       </c>
       <c r="G31" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>0.97674418604651159</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>1.6976744186046511</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>1.2093023255813955</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="G33" s="5" t="s">
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="G33" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
@@ -4351,15 +5234,15 @@
         <v>0.59</v>
       </c>
       <c r="G35" s="1">
-        <f t="shared" ref="G35:I37" si="10">+C35/$B35</f>
+        <f t="shared" ref="G35:I37" si="5">+C35/$B35</f>
         <v>2.3043478260869565</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>0.97826086956521741</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>1.2826086956521738</v>
       </c>
     </row>
@@ -4380,15 +5263,15 @@
         <v>0.48</v>
       </c>
       <c r="G36" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>4.0384615384615383</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>2.0384615384615383</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>1.846153846153846</v>
       </c>
     </row>
@@ -4409,32 +5292,32 @@
         <v>0.5</v>
       </c>
       <c r="G37" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>1.9795918367346939</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>1.0816326530612246</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>1.0204081632653061</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G15:I15"/>
     <mergeCell ref="A21:E21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="A27:E27"/>
     <mergeCell ref="G27:I27"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="G33:I33"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G15:I15"/>
   </mergeCells>
   <conditionalFormatting sqref="I17:I20">
     <cfRule type="colorScale" priority="15">

</xml_diff>